<commit_message>
RUH 21-APR-2024. Codes Update
</commit_message>
<xml_diff>
--- a/Applied_WebApplication/wwwroot/PrintedReports/StockInHand.xlsx
+++ b/Applied_WebApplication/wwwroot/PrintedReports/StockInHand.xlsx
@@ -285,7 +285,7 @@
       </c>
       <c s="3" t="inlineStr" r="B6">
         <is>
-          <t xml:space="preserve">Stock Titlre</t>
+          <t xml:space="preserve">Stock Title</t>
         </is>
       </c>
       <c s="3" t="inlineStr" r="C6">
@@ -1792,7 +1792,7 @@
         <v>48891086.40</v>
       </c>
       <c s="8" r="L36">
-        <v>8150.89</v>
+        <v>45.90</v>
       </c>
     </row>
     <row r="37" ht="0.05" customHeight="1"/>

</xml_diff>